<commit_message>
Minor changes in excel
</commit_message>
<xml_diff>
--- a/TelaDocTest/src/main/java/com/teladoc/qa/testdata/ExcelTestData.xlsx
+++ b/TelaDocTest/src/main/java/com/teladoc/qa/testdata/ExcelTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rupalidash/Rupali-personal/TelaDocTest/src/main/java/com/teladoc/qa/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rupalidash/git/Rupali_Dash_teladoc_challenge/TelaDocTest/src/main/java/com/teladoc/qa/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630495D7-3D01-5F4F-A6CA-E4A0B790750D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591A5A0A-4EB8-9A4E-A0D7-465F0CE8E189}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="3180" windowWidth="27240" windowHeight="16440" xr2:uid="{6E63AEB0-C48A-484B-85A5-279D48D4EC38}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>firstname</t>
   </si>
@@ -60,9 +60,6 @@
     <t>testUser@bw.com</t>
   </si>
   <si>
-    <t>5#$#(&amp;</t>
-  </si>
-  <si>
     <t>cellphone</t>
   </si>
   <si>
@@ -73,6 +70,12 @@
   </si>
   <si>
     <t>SampleTestUser</t>
+  </si>
+  <si>
+    <t>1219234</t>
+  </si>
+  <si>
+    <t>35#$#(&amp;</t>
   </si>
 </sst>
 </file>
@@ -122,11 +125,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,7 +446,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,21 +475,21 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
@@ -495,8 +497,8 @@
       <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3">
-        <v>111222</v>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>